<commit_message>
cierre 21 Mar 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #03  MARZO  2022/BALANCE    ZAVALETA   MARZO  2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #03  MARZO  2022/BALANCE    ZAVALETA   MARZO  2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="0" windowWidth="16605" windowHeight="10920" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="3690" yWindow="0" windowWidth="16605" windowHeight="10920" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="OCTUBRE      2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -457,7 +457,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="587">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -2200,6 +2200,24 @@
   </si>
   <si>
     <t>SALCHICHA</t>
+  </si>
+  <si>
+    <t>Comisiones BANCO</t>
+  </si>
+  <si>
+    <t>FEBRERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMISION </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BANCARAI </t>
+  </si>
+  <si>
+    <t>QUESOS GOUDA</t>
+  </si>
+  <si>
+    <t>POLLO-JAMONES-QUESOS-MIXIOTES-CHISTORRA</t>
   </si>
 </sst>
 </file>
@@ -4099,7 +4117,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="596">
+  <cellXfs count="597">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -5077,6 +5095,9 @@
     <xf numFmtId="44" fontId="3" fillId="6" borderId="89" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8399,23 +8420,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="511"/>
-      <c r="C1" s="513" t="s">
+      <c r="B1" s="512"/>
+      <c r="C1" s="514" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
-      <c r="K1" s="514"/>
-      <c r="L1" s="514"/>
-      <c r="M1" s="514"/>
+      <c r="D1" s="515"/>
+      <c r="E1" s="515"/>
+      <c r="F1" s="515"/>
+      <c r="G1" s="515"/>
+      <c r="H1" s="515"/>
+      <c r="I1" s="515"/>
+      <c r="J1" s="515"/>
+      <c r="K1" s="515"/>
+      <c r="L1" s="515"/>
+      <c r="M1" s="515"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="512"/>
+      <c r="B2" s="513"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -8425,17 +8446,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="515" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="516"/>
+      <c r="B3" s="516" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="517"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="517" t="s">
+      <c r="H3" s="518" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="517"/>
+      <c r="I3" s="518"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -8449,14 +8470,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="518" t="s">
+      <c r="E4" s="519" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="519"/>
-      <c r="H4" s="520" t="s">
+      <c r="F4" s="520"/>
+      <c r="H4" s="521" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="521"/>
+      <c r="I4" s="522"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -8466,10 +8487,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="492" t="s">
+      <c r="P4" s="493" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="493"/>
+      <c r="Q4" s="494"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -9910,11 +9931,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="494">
+      <c r="M39" s="495">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="496">
+      <c r="N39" s="497">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -9940,8 +9961,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="495"/>
-      <c r="N40" s="497"/>
+      <c r="M40" s="496"/>
+      <c r="N40" s="498"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -10156,29 +10177,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="498" t="s">
+      <c r="H52" s="499" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="499"/>
+      <c r="I52" s="500"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="500">
+      <c r="K52" s="501">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="501"/>
-      <c r="M52" s="502">
+      <c r="L52" s="502"/>
+      <c r="M52" s="503">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="503"/>
+      <c r="N52" s="504"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="504" t="s">
+      <c r="D53" s="505" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="504"/>
+      <c r="E53" s="505"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -10189,22 +10210,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="504" t="s">
+      <c r="D54" s="505" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="504"/>
+      <c r="E54" s="505"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="505" t="s">
+      <c r="I54" s="506" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="506"/>
-      <c r="K54" s="507">
+      <c r="J54" s="507"/>
+      <c r="K54" s="508">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="508"/>
+      <c r="L54" s="509"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -10237,11 +10258,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="509">
+      <c r="K56" s="510">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="510"/>
+      <c r="L56" s="511"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -10258,22 +10279,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="487" t="s">
+      <c r="D58" s="488" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="488"/>
+      <c r="E58" s="489"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="489" t="s">
+      <c r="I58" s="490" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="490"/>
-      <c r="K58" s="491">
+      <c r="J58" s="491"/>
+      <c r="K58" s="492">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="491"/>
+      <c r="L58" s="492"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -12777,7 +12798,7 @@
       <c r="C80" s="214"/>
       <c r="D80" s="256"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="549" t="s">
+      <c r="F80" s="550" t="s">
         <v>207</v>
       </c>
       <c r="K80" s="1"/>
@@ -12792,7 +12813,7 @@
       <c r="C81" s="477"/>
       <c r="D81" s="478"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="550"/>
+      <c r="F81" s="551"/>
       <c r="K81" s="1"/>
       <c r="L81" s="97"/>
       <c r="M81" s="3"/>
@@ -13074,8 +13095,8 @@
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13104,23 +13125,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="511"/>
-      <c r="C1" s="553" t="s">
+      <c r="B1" s="512"/>
+      <c r="C1" s="554" t="s">
         <v>458</v>
       </c>
-      <c r="D1" s="554"/>
-      <c r="E1" s="554"/>
-      <c r="F1" s="554"/>
-      <c r="G1" s="554"/>
-      <c r="H1" s="554"/>
-      <c r="I1" s="554"/>
-      <c r="J1" s="554"/>
-      <c r="K1" s="554"/>
-      <c r="L1" s="554"/>
-      <c r="M1" s="554"/>
+      <c r="D1" s="555"/>
+      <c r="E1" s="555"/>
+      <c r="F1" s="555"/>
+      <c r="G1" s="555"/>
+      <c r="H1" s="555"/>
+      <c r="I1" s="555"/>
+      <c r="J1" s="555"/>
+      <c r="K1" s="555"/>
+      <c r="L1" s="555"/>
+      <c r="M1" s="555"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="512"/>
+      <c r="B2" s="513"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -13130,24 +13151,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="515" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="516"/>
+      <c r="B3" s="516" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="517"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="517" t="s">
+      <c r="H3" s="518" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="517"/>
+      <c r="I3" s="518"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="541" t="s">
+      <c r="P3" s="542" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="551" t="s">
+      <c r="R3" s="552" t="s">
         <v>216</v>
       </c>
     </row>
@@ -13162,14 +13183,14 @@
       <c r="D4" s="18">
         <v>44619</v>
       </c>
-      <c r="E4" s="518" t="s">
+      <c r="E4" s="519" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="519"/>
-      <c r="H4" s="520" t="s">
+      <c r="F4" s="520"/>
+      <c r="H4" s="521" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="521"/>
+      <c r="I4" s="522"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -13179,15 +13200,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="542"/>
+      <c r="P4" s="543"/>
       <c r="Q4" s="323" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="552"/>
-      <c r="W4" s="524" t="s">
+      <c r="R4" s="553"/>
+      <c r="W4" s="525" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="524"/>
+      <c r="X4" s="525"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -13238,8 +13259,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="325"/>
-      <c r="W5" s="524"/>
-      <c r="X5" s="524"/>
+      <c r="W5" s="525"/>
+      <c r="X5" s="525"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -14002,7 +14023,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="528">
+      <c r="W19" s="529">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -14054,7 +14075,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="529"/>
+      <c r="W20" s="530"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -14063,29 +14084,37 @@
       <c r="B21" s="24">
         <v>44636</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="35"/>
+      <c r="C21" s="25">
+        <v>18610</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>586</v>
+      </c>
       <c r="E21" s="27">
         <v>44636</v>
       </c>
-      <c r="F21" s="28"/>
+      <c r="F21" s="28">
+        <v>116930</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="36">
         <v>44636</v>
       </c>
-      <c r="I21" s="30"/>
+      <c r="I21" s="30">
+        <v>1391</v>
+      </c>
       <c r="J21" s="37"/>
       <c r="K21" s="48"/>
       <c r="L21" s="45"/>
       <c r="M21" s="32">
-        <v>0</v>
+        <v>65434</v>
       </c>
       <c r="N21" s="33">
-        <v>0</v>
+        <v>31495</v>
       </c>
       <c r="P21" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>116930</v>
       </c>
       <c r="Q21" s="326">
         <f t="shared" si="1"/>
@@ -14095,8 +14124,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="530"/>
-      <c r="X21" s="530"/>
+      <c r="W21" s="531"/>
+      <c r="X21" s="531"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -14179,8 +14208,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="531"/>
-      <c r="X23" s="531"/>
+      <c r="W23" s="532"/>
+      <c r="X23" s="532"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -14221,8 +14250,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="531"/>
-      <c r="X24" s="531"/>
+      <c r="W24" s="532"/>
+      <c r="X24" s="532"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -14262,8 +14291,8 @@
       <c r="R25" s="320">
         <v>0</v>
       </c>
-      <c r="W25" s="532"/>
-      <c r="X25" s="532"/>
+      <c r="W25" s="533"/>
+      <c r="X25" s="533"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -14304,8 +14333,8 @@
       <c r="R26" s="320">
         <v>0</v>
       </c>
-      <c r="W26" s="532"/>
-      <c r="X26" s="532"/>
+      <c r="W26" s="533"/>
+      <c r="X26" s="533"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -14346,9 +14375,9 @@
       <c r="R27" s="320">
         <v>0</v>
       </c>
-      <c r="W27" s="525"/>
-      <c r="X27" s="526"/>
-      <c r="Y27" s="527"/>
+      <c r="W27" s="526"/>
+      <c r="X27" s="527"/>
+      <c r="Y27" s="528"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -14388,9 +14417,9 @@
       <c r="R28" s="320">
         <v>0</v>
       </c>
-      <c r="W28" s="526"/>
-      <c r="X28" s="526"/>
-      <c r="Y28" s="527"/>
+      <c r="W28" s="527"/>
+      <c r="X28" s="527"/>
+      <c r="Y28" s="528"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -14663,12 +14692,12 @@
       <c r="N35" s="268">
         <v>0</v>
       </c>
-      <c r="P35" s="34">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="438">
+      <c r="P35" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q35" s="438" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R35" s="228"/>
     </row>
@@ -14691,21 +14720,21 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="543">
+      <c r="M36" s="544">
         <f>SUM(M5:M35)</f>
-        <v>736637.66</v>
-      </c>
-      <c r="N36" s="545">
+        <v>802071.66</v>
+      </c>
+      <c r="N36" s="546">
         <f>SUM(N5:N35)</f>
-        <v>442985</v>
+        <v>474480</v>
       </c>
       <c r="O36" s="276"/>
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="570">
+      <c r="Q36" s="571" t="e">
         <f>SUM(Q5:Q35)</f>
-        <v>1.5900000000256114</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R36" s="228"/>
     </row>
@@ -14728,13 +14757,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="544"/>
-      <c r="N37" s="546"/>
+      <c r="M37" s="545"/>
+      <c r="N37" s="547"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="571"/>
+      <c r="Q37" s="572"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -14784,14 +14813,14 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="572">
+      <c r="M39" s="573">
         <f>M36+N36</f>
-        <v>1179622.6600000001</v>
-      </c>
-      <c r="N39" s="573"/>
+        <v>1276551.6600000001</v>
+      </c>
+      <c r="N39" s="574"/>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
-        <v>1514811.59</v>
+        <v>1631741.59</v>
       </c>
       <c r="Q39" s="275"/>
     </row>
@@ -14994,7 +15023,7 @@
       </c>
       <c r="C50" s="87">
         <f>SUM(C5:C49)</f>
-        <v>246913</v>
+        <v>265523</v>
       </c>
       <c r="D50" s="88"/>
       <c r="E50" s="89" t="s">
@@ -15002,7 +15031,7 @@
       </c>
       <c r="F50" s="90">
         <f>SUM(F5:F49)</f>
-        <v>1472641</v>
+        <v>1589571</v>
       </c>
       <c r="G50" s="88"/>
       <c r="H50" s="91" t="s">
@@ -15010,7 +15039,7 @@
       </c>
       <c r="I50" s="92">
         <f>SUM(I5:I49)</f>
-        <v>58112.5</v>
+        <v>59503.5</v>
       </c>
       <c r="J50" s="93"/>
       <c r="K50" s="94" t="s">
@@ -15036,50 +15065,50 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="498" t="s">
+      <c r="H52" s="499" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="499"/>
+      <c r="I52" s="500"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="500">
+      <c r="K52" s="501">
         <f>I50+L50</f>
-        <v>119219.69</v>
-      </c>
-      <c r="L52" s="533"/>
+        <v>120610.69</v>
+      </c>
+      <c r="L52" s="534"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="504" t="s">
+      <c r="D53" s="505" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="504"/>
+      <c r="E53" s="505"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
-        <v>1106508.31</v>
+        <v>1203437.31</v>
       </c>
       <c r="I53" s="102"/>
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="534" t="s">
+      <c r="D54" s="535" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="534"/>
+      <c r="E54" s="535"/>
       <c r="F54" s="111">
         <v>0</v>
       </c>
-      <c r="I54" s="505" t="s">
+      <c r="I54" s="506" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="506"/>
-      <c r="K54" s="507">
+      <c r="J54" s="507"/>
+      <c r="K54" s="508">
         <f>F56+F57+F58</f>
-        <v>1106508.31</v>
-      </c>
-      <c r="L54" s="507"/>
+        <v>1203437.31</v>
+      </c>
+      <c r="L54" s="508"/>
       <c r="M54" s="422"/>
       <c r="N54" s="422"/>
       <c r="O54" s="422"/>
@@ -15113,18 +15142,18 @@
       </c>
       <c r="F56" s="96">
         <f>SUM(F53:F55)</f>
-        <v>1106508.31</v>
+        <v>1203437.31</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="509">
+      <c r="K56" s="510">
         <f>-C4</f>
         <v>-1266568.45</v>
       </c>
-      <c r="L56" s="510"/>
+      <c r="L56" s="511"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -15141,22 +15170,22 @@
       <c r="C58" s="112">
         <v>44619</v>
       </c>
-      <c r="D58" s="487" t="s">
+      <c r="D58" s="488" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="488"/>
+      <c r="E58" s="489"/>
       <c r="F58" s="113">
         <v>0</v>
       </c>
-      <c r="I58" s="489" t="s">
+      <c r="I58" s="490" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="490"/>
-      <c r="K58" s="491">
+      <c r="J58" s="491"/>
+      <c r="K58" s="492">
         <f>K54+K56</f>
-        <v>-160060.1399999999</v>
-      </c>
-      <c r="L58" s="491"/>
+        <v>-63131.139999999898</v>
+      </c>
+      <c r="L58" s="492"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -17140,7 +17169,7 @@
       <c r="C80" s="214"/>
       <c r="D80" s="256"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="549" t="s">
+      <c r="F80" s="550" t="s">
         <v>207</v>
       </c>
       <c r="K80" s="1"/>
@@ -17153,7 +17182,7 @@
       <c r="C81" s="1"/>
       <c r="D81" s="256"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="550"/>
+      <c r="F81" s="551"/>
       <c r="K81" s="1"/>
       <c r="L81" s="97"/>
       <c r="M81" s="3"/>
@@ -17462,11 +17491,11 @@
   <sheetData>
     <row r="1" spans="2:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="155"/>
-      <c r="C1" s="580" t="s">
+      <c r="C1" s="581" t="s">
         <v>320</v>
       </c>
-      <c r="D1" s="580"/>
-      <c r="E1" s="581"/>
+      <c r="D1" s="581"/>
+      <c r="E1" s="582"/>
       <c r="F1" s="386"/>
     </row>
     <row r="2" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -17484,12 +17513,12 @@
       <c r="F3" s="393"/>
     </row>
     <row r="4" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="582" t="s">
+      <c r="B4" s="583" t="s">
         <v>316</v>
       </c>
-      <c r="C4" s="583"/>
-      <c r="D4" s="583"/>
-      <c r="E4" s="583"/>
+      <c r="C4" s="584"/>
+      <c r="D4" s="584"/>
+      <c r="E4" s="584"/>
       <c r="F4" s="394">
         <v>499853.16</v>
       </c>
@@ -17504,12 +17533,12 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B6" s="584" t="s">
+      <c r="B6" s="585" t="s">
         <v>317</v>
       </c>
-      <c r="C6" s="585"/>
-      <c r="D6" s="585"/>
-      <c r="E6" s="585"/>
+      <c r="C6" s="586"/>
+      <c r="D6" s="586"/>
+      <c r="E6" s="586"/>
       <c r="F6" s="394">
         <v>781251.72</v>
       </c>
@@ -17527,10 +17556,10 @@
       <c r="B8" s="387"/>
       <c r="C8" s="380"/>
       <c r="D8" s="381"/>
-      <c r="E8" s="586" t="s">
+      <c r="E8" s="587" t="s">
         <v>315</v>
       </c>
-      <c r="F8" s="588">
+      <c r="F8" s="589">
         <f>SUM(F4:F7)</f>
         <v>1281104.8799999999</v>
       </c>
@@ -17539,8 +17568,8 @@
       <c r="B9" s="387"/>
       <c r="C9" s="380"/>
       <c r="D9" s="381"/>
-      <c r="E9" s="587"/>
-      <c r="F9" s="589"/>
+      <c r="E9" s="588"/>
+      <c r="F9" s="590"/>
     </row>
     <row r="10" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="387"/>
@@ -17564,12 +17593,12 @@
       <c r="F12" s="393"/>
     </row>
     <row r="13" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B13" s="590" t="s">
+      <c r="B13" s="591" t="s">
         <v>318</v>
       </c>
-      <c r="C13" s="591"/>
-      <c r="D13" s="591"/>
-      <c r="E13" s="591"/>
+      <c r="C13" s="592"/>
+      <c r="D13" s="592"/>
+      <c r="E13" s="592"/>
       <c r="F13" s="394">
         <v>255460.4</v>
       </c>
@@ -17584,12 +17613,12 @@
       </c>
     </row>
     <row r="15" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="590" t="s">
+      <c r="B15" s="591" t="s">
         <v>319</v>
       </c>
-      <c r="C15" s="591"/>
-      <c r="D15" s="591"/>
-      <c r="E15" s="591"/>
+      <c r="C15" s="592"/>
+      <c r="D15" s="592"/>
+      <c r="E15" s="592"/>
       <c r="F15" s="394">
         <v>6037.34</v>
       </c>
@@ -17607,10 +17636,10 @@
       <c r="B17" s="387"/>
       <c r="C17" s="380"/>
       <c r="D17" s="381"/>
-      <c r="E17" s="592" t="s">
+      <c r="E17" s="593" t="s">
         <v>315</v>
       </c>
-      <c r="F17" s="594">
+      <c r="F17" s="595">
         <f>SUM(F13:F16)</f>
         <v>261497.74</v>
       </c>
@@ -17619,8 +17648,8 @@
       <c r="B18" s="387"/>
       <c r="C18" s="380"/>
       <c r="D18" s="381"/>
-      <c r="E18" s="593"/>
-      <c r="F18" s="595"/>
+      <c r="E18" s="594"/>
+      <c r="F18" s="596"/>
     </row>
     <row r="19" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="387"/>
@@ -17644,22 +17673,22 @@
       <c r="F21" s="393"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="574" t="s">
+      <c r="B22" s="575" t="s">
         <v>321</v>
       </c>
-      <c r="C22" s="575"/>
-      <c r="D22" s="575"/>
-      <c r="E22" s="575"/>
-      <c r="F22" s="578">
+      <c r="C22" s="576"/>
+      <c r="D22" s="576"/>
+      <c r="E22" s="576"/>
+      <c r="F22" s="579">
         <v>12020</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="576"/>
-      <c r="C23" s="577"/>
-      <c r="D23" s="577"/>
-      <c r="E23" s="577"/>
-      <c r="F23" s="579"/>
+      <c r="B23" s="577"/>
+      <c r="C23" s="578"/>
+      <c r="D23" s="578"/>
+      <c r="E23" s="578"/>
+      <c r="F23" s="580"/>
     </row>
     <row r="24" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="355"/>
@@ -19019,7 +19048,7 @@
       <c r="A41" s="140">
         <v>44507</v>
       </c>
-      <c r="B41" s="522" t="s">
+      <c r="B41" s="523" t="s">
         <v>92</v>
       </c>
       <c r="C41" s="190">
@@ -19051,7 +19080,7 @@
       <c r="A42" s="140" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="523"/>
+      <c r="B42" s="524"/>
       <c r="C42" s="143">
         <v>0</v>
       </c>
@@ -20647,23 +20676,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="511"/>
-      <c r="C1" s="513" t="s">
+      <c r="B1" s="512"/>
+      <c r="C1" s="514" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
-      <c r="K1" s="514"/>
-      <c r="L1" s="514"/>
-      <c r="M1" s="514"/>
+      <c r="D1" s="515"/>
+      <c r="E1" s="515"/>
+      <c r="F1" s="515"/>
+      <c r="G1" s="515"/>
+      <c r="H1" s="515"/>
+      <c r="I1" s="515"/>
+      <c r="J1" s="515"/>
+      <c r="K1" s="515"/>
+      <c r="L1" s="515"/>
+      <c r="M1" s="515"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="512"/>
+      <c r="B2" s="513"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -20673,21 +20702,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="515" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="516"/>
+      <c r="B3" s="516" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="517"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="517" t="s">
+      <c r="H3" s="518" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="517"/>
+      <c r="I3" s="518"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="541" t="s">
+      <c r="P3" s="542" t="s">
         <v>6</v>
       </c>
     </row>
@@ -20702,14 +20731,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="518" t="s">
+      <c r="E4" s="519" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="519"/>
-      <c r="H4" s="520" t="s">
+      <c r="F4" s="520"/>
+      <c r="H4" s="521" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="521"/>
+      <c r="I4" s="522"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -20719,14 +20748,14 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="542"/>
+      <c r="P4" s="543"/>
       <c r="Q4" s="286" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="524" t="s">
+      <c r="W4" s="525" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="524"/>
+      <c r="X4" s="525"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -20777,8 +20806,8 @@
         <f>20000+7936</f>
         <v>27936</v>
       </c>
-      <c r="W5" s="524"/>
-      <c r="X5" s="524"/>
+      <c r="W5" s="525"/>
+      <c r="X5" s="525"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -21549,7 +21578,7 @@
         <v>26370</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="528">
+      <c r="W19" s="529">
         <f>SUM(W6:W18)</f>
         <v>935136</v>
       </c>
@@ -21601,7 +21630,7 @@
         <v>16395.830000000002</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="529"/>
+      <c r="W20" s="530"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -21650,8 +21679,8 @@
         <v>19188.82</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="530"/>
-      <c r="X21" s="530"/>
+      <c r="W21" s="531"/>
+      <c r="X21" s="531"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -21752,8 +21781,8 @@
         <v>45217.29</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="531"/>
-      <c r="X23" s="531"/>
+      <c r="W23" s="532"/>
+      <c r="X23" s="532"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -21807,8 +21836,8 @@
         <v>23159.17</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="531"/>
-      <c r="X24" s="531"/>
+      <c r="W24" s="532"/>
+      <c r="X24" s="532"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -21854,8 +21883,8 @@
       <c r="R25" s="285">
         <v>28952</v>
       </c>
-      <c r="W25" s="532"/>
-      <c r="X25" s="532"/>
+      <c r="W25" s="533"/>
+      <c r="X25" s="533"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -21906,8 +21935,8 @@
       <c r="R26" s="285">
         <v>21771.5</v>
       </c>
-      <c r="W26" s="532"/>
-      <c r="X26" s="532"/>
+      <c r="W26" s="533"/>
+      <c r="X26" s="533"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -21955,9 +21984,9 @@
       <c r="R27" s="285">
         <v>14637</v>
       </c>
-      <c r="W27" s="525"/>
-      <c r="X27" s="526"/>
-      <c r="Y27" s="527"/>
+      <c r="W27" s="526"/>
+      <c r="X27" s="527"/>
+      <c r="Y27" s="528"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -22007,9 +22036,9 @@
       <c r="R28" s="285">
         <v>0</v>
       </c>
-      <c r="W28" s="526"/>
-      <c r="X28" s="526"/>
-      <c r="Y28" s="527"/>
+      <c r="W28" s="527"/>
+      <c r="X28" s="527"/>
+      <c r="Y28" s="528"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -22344,11 +22373,11 @@
       <c r="L36" s="44">
         <v>5940</v>
       </c>
-      <c r="M36" s="543">
+      <c r="M36" s="544">
         <f>SUM(M5:M35)</f>
         <v>321168.83</v>
       </c>
-      <c r="N36" s="545">
+      <c r="N36" s="546">
         <f>SUM(N5:N35)</f>
         <v>467016</v>
       </c>
@@ -22356,7 +22385,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="547">
+      <c r="Q36" s="548">
         <f>SUM(Q5:Q35)</f>
         <v>-637069.14000000013</v>
       </c>
@@ -22391,13 +22420,13 @@
       <c r="L37" s="61">
         <v>7929.62</v>
       </c>
-      <c r="M37" s="544"/>
-      <c r="N37" s="546"/>
+      <c r="M37" s="545"/>
+      <c r="N37" s="547"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="548"/>
+      <c r="Q37" s="549"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -22687,26 +22716,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="498" t="s">
+      <c r="H52" s="499" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="499"/>
+      <c r="I52" s="500"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="500">
+      <c r="K52" s="501">
         <f>I50+L50</f>
         <v>71911.59</v>
       </c>
-      <c r="L52" s="533"/>
+      <c r="L52" s="534"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="504" t="s">
+      <c r="D53" s="505" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="504"/>
+      <c r="E53" s="505"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
         <v>-25952.549999999814</v>
@@ -22715,29 +22744,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="534" t="s">
+      <c r="D54" s="535" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="534"/>
+      <c r="E54" s="535"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="505" t="s">
+      <c r="I54" s="506" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="506"/>
-      <c r="K54" s="507">
+      <c r="J54" s="507"/>
+      <c r="K54" s="508">
         <f>F56+F57+F58</f>
         <v>1308778.3500000003</v>
       </c>
-      <c r="L54" s="507"/>
-      <c r="M54" s="535" t="s">
+      <c r="L54" s="508"/>
+      <c r="M54" s="536" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="536"/>
-      <c r="O54" s="536"/>
-      <c r="P54" s="536"/>
-      <c r="Q54" s="537"/>
+      <c r="N54" s="537"/>
+      <c r="O54" s="537"/>
+      <c r="P54" s="537"/>
+      <c r="Q54" s="538"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="314" t="s">
@@ -22751,11 +22780,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="538"/>
-      <c r="N55" s="539"/>
-      <c r="O55" s="539"/>
-      <c r="P55" s="539"/>
-      <c r="Q55" s="540"/>
+      <c r="M55" s="539"/>
+      <c r="N55" s="540"/>
+      <c r="O55" s="540"/>
+      <c r="P55" s="540"/>
+      <c r="Q55" s="541"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -22773,11 +22802,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="509">
+      <c r="K56" s="510">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="510"/>
+      <c r="L56" s="511"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -22794,22 +22823,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="487" t="s">
+      <c r="D58" s="488" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="488"/>
+      <c r="E58" s="489"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="489" t="s">
+      <c r="I58" s="490" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="490"/>
-      <c r="K58" s="491">
+      <c r="J58" s="491"/>
+      <c r="K58" s="492">
         <f>K54+K56</f>
         <v>741389.00000000035</v>
       </c>
-      <c r="L58" s="491"/>
+      <c r="L58" s="492"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -25399,7 +25428,7 @@
       <c r="C87" s="214"/>
       <c r="D87" s="97"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="549" t="s">
+      <c r="F87" s="550" t="s">
         <v>207</v>
       </c>
       <c r="K87" s="1"/>
@@ -25412,7 +25441,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="97"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="550"/>
+      <c r="F88" s="551"/>
       <c r="K88" s="1"/>
       <c r="L88" s="256"/>
       <c r="M88" s="3"/>
@@ -25694,8 +25723,8 @@
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -25724,23 +25753,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="511"/>
-      <c r="C1" s="513" t="s">
+      <c r="B1" s="512"/>
+      <c r="C1" s="514" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="514"/>
-      <c r="E1" s="514"/>
-      <c r="F1" s="514"/>
-      <c r="G1" s="514"/>
-      <c r="H1" s="514"/>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
-      <c r="K1" s="514"/>
-      <c r="L1" s="514"/>
-      <c r="M1" s="514"/>
+      <c r="D1" s="515"/>
+      <c r="E1" s="515"/>
+      <c r="F1" s="515"/>
+      <c r="G1" s="515"/>
+      <c r="H1" s="515"/>
+      <c r="I1" s="515"/>
+      <c r="J1" s="515"/>
+      <c r="K1" s="515"/>
+      <c r="L1" s="515"/>
+      <c r="M1" s="515"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="512"/>
+      <c r="B2" s="513"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -25750,24 +25779,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="515" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="516"/>
+      <c r="B3" s="516" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="517"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="517" t="s">
+      <c r="H3" s="518" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="517"/>
+      <c r="I3" s="518"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="541" t="s">
+      <c r="P3" s="542" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="551" t="s">
+      <c r="R3" s="552" t="s">
         <v>216</v>
       </c>
     </row>
@@ -25782,14 +25811,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="518" t="s">
+      <c r="E4" s="519" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="519"/>
-      <c r="H4" s="520" t="s">
+      <c r="F4" s="520"/>
+      <c r="H4" s="521" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="521"/>
+      <c r="I4" s="522"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -25799,15 +25828,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="542"/>
+      <c r="P4" s="543"/>
       <c r="Q4" s="323" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="552"/>
-      <c r="W4" s="524" t="s">
+      <c r="R4" s="553"/>
+      <c r="W4" s="525" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="524"/>
+      <c r="X4" s="525"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -25868,8 +25897,8 @@
       <c r="S5" s="325" t="s">
         <v>213</v>
       </c>
-      <c r="W5" s="524"/>
-      <c r="X5" s="524"/>
+      <c r="W5" s="525"/>
+      <c r="X5" s="525"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -26626,7 +26655,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="528">
+      <c r="W19" s="529">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -26678,7 +26707,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="529"/>
+      <c r="W20" s="530"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -26727,8 +26756,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="530"/>
-      <c r="X21" s="530"/>
+      <c r="W21" s="531"/>
+      <c r="X21" s="531"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -26829,8 +26858,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="531"/>
-      <c r="X23" s="531"/>
+      <c r="W23" s="532"/>
+      <c r="X23" s="532"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -26881,8 +26910,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="531"/>
-      <c r="X24" s="531"/>
+      <c r="W24" s="532"/>
+      <c r="X24" s="532"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -26928,8 +26957,8 @@
       <c r="R25" s="320">
         <v>0</v>
       </c>
-      <c r="W25" s="532"/>
-      <c r="X25" s="532"/>
+      <c r="W25" s="533"/>
+      <c r="X25" s="533"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -26977,8 +27006,8 @@
       <c r="R26" s="320">
         <v>0</v>
       </c>
-      <c r="W26" s="532"/>
-      <c r="X26" s="532"/>
+      <c r="W26" s="533"/>
+      <c r="X26" s="533"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -27038,9 +27067,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="525"/>
-      <c r="X27" s="526"/>
-      <c r="Y27" s="527"/>
+      <c r="W27" s="526"/>
+      <c r="X27" s="527"/>
+      <c r="Y27" s="528"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -27094,9 +27123,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="526"/>
-      <c r="X28" s="526"/>
-      <c r="Y28" s="527"/>
+      <c r="W28" s="527"/>
+      <c r="X28" s="527"/>
+      <c r="Y28" s="528"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -27412,11 +27441,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="543">
+      <c r="M36" s="544">
         <f>SUM(M5:M35)</f>
         <v>1077791.3</v>
       </c>
-      <c r="N36" s="545">
+      <c r="N36" s="546">
         <f>SUM(N5:N35)</f>
         <v>936398</v>
       </c>
@@ -27424,7 +27453,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="547">
+      <c r="Q36" s="548">
         <f>SUM(Q5:Q35)</f>
         <v>-14262.940000000002</v>
       </c>
@@ -27443,13 +27472,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="544"/>
-      <c r="N37" s="546"/>
+      <c r="M37" s="545"/>
+      <c r="N37" s="547"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="548"/>
+      <c r="Q37" s="549"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -27723,26 +27752,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="498" t="s">
+      <c r="H52" s="499" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="499"/>
+      <c r="I52" s="500"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="500">
+      <c r="K52" s="501">
         <f>I50+L50</f>
         <v>90750.75</v>
       </c>
-      <c r="L52" s="533"/>
+      <c r="L52" s="534"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="504" t="s">
+      <c r="D53" s="505" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="504"/>
+      <c r="E53" s="505"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
         <v>1739855.03</v>
@@ -27751,29 +27780,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="534" t="s">
+      <c r="D54" s="535" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="534"/>
+      <c r="E54" s="535"/>
       <c r="F54" s="111">
         <v>-1567070.66</v>
       </c>
-      <c r="I54" s="505" t="s">
+      <c r="I54" s="506" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="506"/>
-      <c r="K54" s="507">
+      <c r="J54" s="507"/>
+      <c r="K54" s="508">
         <f>F56+F57+F58</f>
         <v>703192.8600000001</v>
       </c>
-      <c r="L54" s="507"/>
-      <c r="M54" s="535" t="s">
+      <c r="L54" s="508"/>
+      <c r="M54" s="536" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="536"/>
-      <c r="O54" s="536"/>
-      <c r="P54" s="536"/>
-      <c r="Q54" s="537"/>
+      <c r="N54" s="537"/>
+      <c r="O54" s="537"/>
+      <c r="P54" s="537"/>
+      <c r="Q54" s="538"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="314" t="s">
@@ -27787,11 +27816,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="538"/>
-      <c r="N55" s="539"/>
-      <c r="O55" s="539"/>
-      <c r="P55" s="539"/>
-      <c r="Q55" s="540"/>
+      <c r="M55" s="539"/>
+      <c r="N55" s="540"/>
+      <c r="O55" s="540"/>
+      <c r="P55" s="540"/>
+      <c r="Q55" s="541"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -27809,11 +27838,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="509">
+      <c r="K56" s="510">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="510"/>
+      <c r="L56" s="511"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -27830,22 +27859,22 @@
       <c r="C58" s="112">
         <v>44563</v>
       </c>
-      <c r="D58" s="487" t="s">
+      <c r="D58" s="488" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="488"/>
+      <c r="E58" s="489"/>
       <c r="F58" s="113">
         <v>754143.23</v>
       </c>
-      <c r="I58" s="489" t="s">
+      <c r="I58" s="490" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="490"/>
-      <c r="K58" s="491">
+      <c r="J58" s="491"/>
+      <c r="K58" s="492">
         <f>K54+K56</f>
         <v>135803.51000000013</v>
       </c>
-      <c r="L58" s="491"/>
+      <c r="L58" s="492"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -30408,7 +30437,7 @@
       <c r="C75" s="214"/>
       <c r="D75" s="256"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="549" t="s">
+      <c r="F75" s="550" t="s">
         <v>207</v>
       </c>
       <c r="K75" s="1"/>
@@ -30421,7 +30450,7 @@
       <c r="C76" s="1"/>
       <c r="D76" s="256"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="550"/>
+      <c r="F76" s="551"/>
       <c r="K76" s="1"/>
       <c r="L76" s="256"/>
       <c r="M76" s="3"/>
@@ -30683,8 +30712,8 @@
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -30713,23 +30742,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="511"/>
-      <c r="C1" s="553" t="s">
+      <c r="B1" s="512"/>
+      <c r="C1" s="554" t="s">
         <v>323</v>
       </c>
-      <c r="D1" s="554"/>
-      <c r="E1" s="554"/>
-      <c r="F1" s="554"/>
-      <c r="G1" s="554"/>
-      <c r="H1" s="554"/>
-      <c r="I1" s="554"/>
-      <c r="J1" s="554"/>
-      <c r="K1" s="554"/>
-      <c r="L1" s="554"/>
-      <c r="M1" s="554"/>
+      <c r="D1" s="555"/>
+      <c r="E1" s="555"/>
+      <c r="F1" s="555"/>
+      <c r="G1" s="555"/>
+      <c r="H1" s="555"/>
+      <c r="I1" s="555"/>
+      <c r="J1" s="555"/>
+      <c r="K1" s="555"/>
+      <c r="L1" s="555"/>
+      <c r="M1" s="555"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="512"/>
+      <c r="B2" s="513"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -30739,24 +30768,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="515" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="516"/>
+      <c r="B3" s="516" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="517"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="517" t="s">
+      <c r="H3" s="518" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="517"/>
+      <c r="I3" s="518"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="541" t="s">
+      <c r="P3" s="542" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="551" t="s">
+      <c r="R3" s="552" t="s">
         <v>216</v>
       </c>
     </row>
@@ -30771,14 +30800,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="518" t="s">
+      <c r="E4" s="519" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="519"/>
-      <c r="H4" s="520" t="s">
+      <c r="F4" s="520"/>
+      <c r="H4" s="521" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="521"/>
+      <c r="I4" s="522"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -30788,15 +30817,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="542"/>
+      <c r="P4" s="543"/>
       <c r="Q4" s="323" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="552"/>
-      <c r="W4" s="524" t="s">
+      <c r="R4" s="553"/>
+      <c r="W4" s="525" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="524"/>
+      <c r="X4" s="525"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -30847,8 +30876,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="325"/>
-      <c r="W5" s="524"/>
-      <c r="X5" s="524"/>
+      <c r="W5" s="525"/>
+      <c r="X5" s="525"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -31612,7 +31641,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="528">
+      <c r="W19" s="529">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -31665,7 +31694,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="529"/>
+      <c r="W20" s="530"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -31714,8 +31743,8 @@
         <v>377273.87</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="530"/>
-      <c r="X21" s="530"/>
+      <c r="W21" s="531"/>
+      <c r="X21" s="531"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -31815,8 +31844,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="531"/>
-      <c r="X23" s="531"/>
+      <c r="W23" s="532"/>
+      <c r="X23" s="532"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -31871,8 +31900,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="531"/>
-      <c r="X24" s="531"/>
+      <c r="W24" s="532"/>
+      <c r="X24" s="532"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -31917,8 +31946,8 @@
       <c r="R25" s="320">
         <v>0</v>
       </c>
-      <c r="W25" s="532"/>
-      <c r="X25" s="532"/>
+      <c r="W25" s="533"/>
+      <c r="X25" s="533"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -31966,8 +31995,8 @@
       <c r="R26" s="320">
         <v>0</v>
       </c>
-      <c r="W26" s="532"/>
-      <c r="X26" s="532"/>
+      <c r="W26" s="533"/>
+      <c r="X26" s="533"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -32021,9 +32050,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="525"/>
-      <c r="X27" s="526"/>
-      <c r="Y27" s="527"/>
+      <c r="W27" s="526"/>
+      <c r="X27" s="527"/>
+      <c r="Y27" s="528"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -32077,9 +32106,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="526"/>
-      <c r="X28" s="526"/>
-      <c r="Y28" s="527"/>
+      <c r="W28" s="527"/>
+      <c r="X28" s="527"/>
+      <c r="Y28" s="528"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -32311,9 +32340,15 @@
     </row>
     <row r="34" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="23"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="64"/>
+      <c r="B34" s="24">
+        <v>44591</v>
+      </c>
+      <c r="C34" s="25">
+        <v>43151.45</v>
+      </c>
+      <c r="D34" s="64" t="s">
+        <v>585</v>
+      </c>
       <c r="E34" s="27"/>
       <c r="F34" s="28"/>
       <c r="G34" s="2"/>
@@ -32384,11 +32419,11 @@
       <c r="L36" s="44">
         <v>13275.84</v>
       </c>
-      <c r="M36" s="543">
+      <c r="M36" s="544">
         <f>SUM(M5:M35)</f>
         <v>1818445.73</v>
       </c>
-      <c r="N36" s="545">
+      <c r="N36" s="546">
         <f>SUM(N5:N35)</f>
         <v>739014</v>
       </c>
@@ -32396,7 +32431,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="547">
+      <c r="Q36" s="548">
         <f>SUM(Q5:Q35)</f>
         <v>-7.2800000000133878</v>
       </c>
@@ -32421,13 +32456,13 @@
       <c r="L37" s="61">
         <v>15060.32</v>
       </c>
-      <c r="M37" s="544"/>
-      <c r="N37" s="546"/>
+      <c r="M37" s="545"/>
+      <c r="N37" s="547"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="548"/>
+      <c r="Q37" s="549"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -32462,9 +32497,15 @@
       <c r="G39" s="2"/>
       <c r="H39" s="36"/>
       <c r="I39" s="71"/>
-      <c r="J39" s="60"/>
-      <c r="K39" s="177"/>
-      <c r="L39" s="61"/>
+      <c r="J39" s="60" t="s">
+        <v>583</v>
+      </c>
+      <c r="K39" s="177" t="s">
+        <v>584</v>
+      </c>
+      <c r="L39" s="61">
+        <v>13803.92</v>
+      </c>
       <c r="M39" s="278"/>
       <c r="N39" s="278"/>
       <c r="P39" s="34">
@@ -32672,7 +32713,7 @@
       </c>
       <c r="C50" s="87">
         <f>SUM(C5:C49)</f>
-        <v>312737.68</v>
+        <v>355889.13</v>
       </c>
       <c r="D50" s="88"/>
       <c r="E50" s="89" t="s">
@@ -32696,7 +32737,7 @@
       </c>
       <c r="L50" s="95">
         <f>SUM(L5:L49)</f>
-        <v>93894.3</v>
+        <v>107698.22</v>
       </c>
       <c r="M50" s="96"/>
       <c r="N50" s="96"/>
@@ -32714,50 +32755,50 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="498" t="s">
+      <c r="H52" s="499" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="499"/>
+      <c r="I52" s="500"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="500">
+      <c r="K52" s="501">
         <f>I50+L50</f>
-        <v>144994.20000000001</v>
-      </c>
-      <c r="L52" s="533"/>
+        <v>158798.12</v>
+      </c>
+      <c r="L52" s="534"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="504" t="s">
+      <c r="D53" s="505" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="504"/>
+      <c r="E53" s="505"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
-        <v>2135426.1199999996</v>
+        <v>2078470.75</v>
       </c>
       <c r="I53" s="102"/>
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="534" t="s">
+      <c r="D54" s="535" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="534"/>
+      <c r="E54" s="535"/>
       <c r="F54" s="111">
         <v>-1448401.2</v>
       </c>
-      <c r="I54" s="505" t="s">
+      <c r="I54" s="506" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="506"/>
-      <c r="K54" s="507">
+      <c r="J54" s="507"/>
+      <c r="K54" s="508">
         <f>F56+F57+F58</f>
-        <v>1082916.0699999996</v>
-      </c>
-      <c r="L54" s="507"/>
+        <v>1025960.7</v>
+      </c>
+      <c r="L54" s="508"/>
       <c r="M54" s="422"/>
       <c r="N54" s="422"/>
       <c r="O54" s="422"/>
@@ -32791,18 +32832,18 @@
       </c>
       <c r="F56" s="96">
         <f>SUM(F53:F55)</f>
-        <v>-221976.34000000032</v>
+        <v>-278931.70999999996</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="509">
+      <c r="K56" s="510">
         <f>-C4</f>
         <v>-754143.23</v>
       </c>
-      <c r="L56" s="510"/>
+      <c r="L56" s="511"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -32819,22 +32860,22 @@
       <c r="C58" s="112">
         <v>44591</v>
       </c>
-      <c r="D58" s="487" t="s">
+      <c r="D58" s="488" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="488"/>
+      <c r="E58" s="489"/>
       <c r="F58" s="113">
         <v>1149740.4099999999</v>
       </c>
-      <c r="I58" s="489" t="s">
+      <c r="I58" s="490" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="490"/>
-      <c r="K58" s="491">
+      <c r="J58" s="491"/>
+      <c r="K58" s="492">
         <f>K54+K56</f>
-        <v>328772.83999999962</v>
-      </c>
-      <c r="L58" s="491"/>
+        <v>271817.46999999997</v>
+      </c>
+      <c r="L58" s="492"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -34677,12 +34718,12 @@
     </row>
     <row r="43" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="245"/>
-      <c r="B43" s="555" t="s">
+      <c r="B43" s="556" t="s">
         <v>420</v>
       </c>
-      <c r="C43" s="556"/>
-      <c r="D43" s="556"/>
-      <c r="E43" s="557"/>
+      <c r="C43" s="557"/>
+      <c r="D43" s="557"/>
+      <c r="E43" s="558"/>
       <c r="F43" s="410">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -34708,10 +34749,10 @@
     </row>
     <row r="44" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="245"/>
-      <c r="B44" s="558"/>
-      <c r="C44" s="559"/>
-      <c r="D44" s="559"/>
-      <c r="E44" s="560"/>
+      <c r="B44" s="559"/>
+      <c r="C44" s="560"/>
+      <c r="D44" s="560"/>
+      <c r="E44" s="561"/>
       <c r="F44" s="410">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -34737,10 +34778,10 @@
     </row>
     <row r="45" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="245"/>
-      <c r="B45" s="561"/>
-      <c r="C45" s="562"/>
-      <c r="D45" s="562"/>
-      <c r="E45" s="563"/>
+      <c r="B45" s="562"/>
+      <c r="C45" s="563"/>
+      <c r="D45" s="563"/>
+      <c r="E45" s="564"/>
       <c r="F45" s="410">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -34815,11 +34856,11 @@
         <v>0</v>
       </c>
       <c r="I48" s="349"/>
-      <c r="J48" s="564" t="s">
+      <c r="J48" s="565" t="s">
         <v>421</v>
       </c>
-      <c r="K48" s="565"/>
-      <c r="L48" s="566"/>
+      <c r="K48" s="566"/>
+      <c r="L48" s="567"/>
       <c r="M48" s="206"/>
       <c r="N48" s="137">
         <f>N47+K48-M48</f>
@@ -34837,9 +34878,9 @@
         <v>0</v>
       </c>
       <c r="I49" s="349"/>
-      <c r="J49" s="567"/>
-      <c r="K49" s="568"/>
-      <c r="L49" s="569"/>
+      <c r="J49" s="568"/>
+      <c r="K49" s="569"/>
+      <c r="L49" s="570"/>
       <c r="M49" s="206"/>
       <c r="N49" s="137">
         <f t="shared" si="1"/>
@@ -35466,7 +35507,7 @@
       <c r="C80" s="214"/>
       <c r="D80" s="256"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="549" t="s">
+      <c r="F80" s="550" t="s">
         <v>207</v>
       </c>
       <c r="K80" s="1"/>
@@ -35479,7 +35520,7 @@
       <c r="C81" s="1"/>
       <c r="D81" s="256"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="550"/>
+      <c r="F81" s="551"/>
       <c r="K81" s="1"/>
       <c r="L81" s="97"/>
       <c r="M81" s="3"/>
@@ -35764,8 +35805,8 @@
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -35794,23 +35835,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="511"/>
-      <c r="C1" s="553" t="s">
+      <c r="B1" s="512"/>
+      <c r="C1" s="554" t="s">
         <v>323</v>
       </c>
-      <c r="D1" s="554"/>
-      <c r="E1" s="554"/>
-      <c r="F1" s="554"/>
-      <c r="G1" s="554"/>
-      <c r="H1" s="554"/>
-      <c r="I1" s="554"/>
-      <c r="J1" s="554"/>
-      <c r="K1" s="554"/>
-      <c r="L1" s="554"/>
-      <c r="M1" s="554"/>
+      <c r="D1" s="555"/>
+      <c r="E1" s="555"/>
+      <c r="F1" s="555"/>
+      <c r="G1" s="555"/>
+      <c r="H1" s="555"/>
+      <c r="I1" s="555"/>
+      <c r="J1" s="555"/>
+      <c r="K1" s="555"/>
+      <c r="L1" s="555"/>
+      <c r="M1" s="555"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="512"/>
+      <c r="B2" s="513"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -35820,24 +35861,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="515" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="516"/>
+      <c r="B3" s="516" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="517"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="517" t="s">
+      <c r="H3" s="518" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="517"/>
+      <c r="I3" s="518"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="541" t="s">
+      <c r="P3" s="542" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="551" t="s">
+      <c r="R3" s="552" t="s">
         <v>216</v>
       </c>
     </row>
@@ -35852,14 +35893,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="518" t="s">
+      <c r="E4" s="519" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="519"/>
-      <c r="H4" s="520" t="s">
+      <c r="F4" s="520"/>
+      <c r="H4" s="521" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="521"/>
+      <c r="I4" s="522"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -35869,15 +35910,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="542"/>
+      <c r="P4" s="543"/>
       <c r="Q4" s="323" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="552"/>
-      <c r="W4" s="524" t="s">
+      <c r="R4" s="553"/>
+      <c r="W4" s="525" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="524"/>
+      <c r="X4" s="525"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -35928,8 +35969,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="325"/>
-      <c r="W5" s="524"/>
-      <c r="X5" s="524"/>
+      <c r="W5" s="525"/>
+      <c r="X5" s="525"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -36690,7 +36731,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="528">
+      <c r="W19" s="529">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -36742,7 +36783,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="529"/>
+      <c r="W20" s="530"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -36791,8 +36832,8 @@
         <v>18072</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="530"/>
-      <c r="X21" s="530"/>
+      <c r="W21" s="531"/>
+      <c r="X21" s="531"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -36891,8 +36932,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="531"/>
-      <c r="X23" s="531"/>
+      <c r="W23" s="532"/>
+      <c r="X23" s="532"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -36947,8 +36988,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="531"/>
-      <c r="X24" s="531"/>
+      <c r="W24" s="532"/>
+      <c r="X24" s="532"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -36996,8 +37037,8 @@
       <c r="R25" s="320">
         <v>0</v>
       </c>
-      <c r="W25" s="532"/>
-      <c r="X25" s="532"/>
+      <c r="W25" s="533"/>
+      <c r="X25" s="533"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -37045,8 +37086,8 @@
       <c r="R26" s="320">
         <v>0</v>
       </c>
-      <c r="W26" s="532"/>
-      <c r="X26" s="532"/>
+      <c r="W26" s="533"/>
+      <c r="X26" s="533"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -37094,9 +37135,9 @@
       <c r="R27" s="320">
         <v>0</v>
       </c>
-      <c r="W27" s="525"/>
-      <c r="X27" s="526"/>
-      <c r="Y27" s="527"/>
+      <c r="W27" s="526"/>
+      <c r="X27" s="527"/>
+      <c r="Y27" s="528"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -37144,9 +37185,9 @@
       <c r="R28" s="320">
         <v>0</v>
       </c>
-      <c r="W28" s="526"/>
-      <c r="X28" s="526"/>
-      <c r="Y28" s="527"/>
+      <c r="W28" s="527"/>
+      <c r="X28" s="527"/>
+      <c r="Y28" s="528"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -37487,11 +37528,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="543">
+      <c r="M36" s="544">
         <f>SUM(M5:M35)</f>
         <v>2143864.4900000002</v>
       </c>
-      <c r="N36" s="545">
+      <c r="N36" s="546">
         <f>SUM(N5:N35)</f>
         <v>791108</v>
       </c>
@@ -37499,7 +37540,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="570">
+      <c r="Q36" s="571">
         <f>SUM(Q5:Q35)</f>
         <v>111.43999999999505</v>
       </c>
@@ -37524,13 +37565,13 @@
       <c r="L37" s="61">
         <v>16518.78</v>
       </c>
-      <c r="M37" s="544"/>
-      <c r="N37" s="546"/>
+      <c r="M37" s="545"/>
+      <c r="N37" s="547"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="571"/>
+      <c r="Q37" s="572"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -37580,11 +37621,11 @@
       <c r="L39" s="61">
         <v>14981.03</v>
       </c>
-      <c r="M39" s="572">
+      <c r="M39" s="573">
         <f>M36+N36</f>
         <v>2934972.49</v>
       </c>
-      <c r="N39" s="573"/>
+      <c r="N39" s="574"/>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
         <v>3450079.65</v>
@@ -37770,9 +37811,15 @@
       <c r="F49" s="72"/>
       <c r="H49" s="83"/>
       <c r="I49" s="77"/>
-      <c r="J49" s="84"/>
-      <c r="K49" s="164"/>
-      <c r="L49" s="9"/>
+      <c r="J49" s="487" t="s">
+        <v>581</v>
+      </c>
+      <c r="K49" s="164" t="s">
+        <v>582</v>
+      </c>
+      <c r="L49" s="9">
+        <v>17279.18</v>
+      </c>
       <c r="M49" s="34"/>
       <c r="N49" s="34"/>
       <c r="P49" s="34"/>
@@ -37808,7 +37855,7 @@
       </c>
       <c r="L50" s="95">
         <f>SUM(L5:L49)</f>
-        <v>114509.62</v>
+        <v>131788.79999999999</v>
       </c>
       <c r="M50" s="96"/>
       <c r="N50" s="96"/>
@@ -37826,50 +37873,50 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="498" t="s">
+      <c r="H52" s="499" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="499"/>
+      <c r="I52" s="500"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="500">
+      <c r="K52" s="501">
         <f>I50+L50</f>
-        <v>180192.62</v>
-      </c>
-      <c r="L52" s="533"/>
+        <v>197471.8</v>
+      </c>
+      <c r="L52" s="534"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="504" t="s">
+      <c r="D53" s="505" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="504"/>
+      <c r="E53" s="505"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
-        <v>2075065.2899999998</v>
+        <v>2057786.11</v>
       </c>
       <c r="I53" s="102"/>
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="534" t="s">
+      <c r="D54" s="535" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="534"/>
+      <c r="E54" s="535"/>
       <c r="F54" s="111">
         <v>-1702928.14</v>
       </c>
-      <c r="I54" s="505" t="s">
+      <c r="I54" s="506" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="506"/>
-      <c r="K54" s="507">
+      <c r="J54" s="507"/>
+      <c r="K54" s="508">
         <f>F56+F57+F58</f>
-        <v>1165244.52</v>
-      </c>
-      <c r="L54" s="507"/>
+        <v>1147965.3400000003</v>
+      </c>
+      <c r="L54" s="508"/>
       <c r="M54" s="422"/>
       <c r="N54" s="422"/>
       <c r="O54" s="422"/>
@@ -37903,18 +37950,18 @@
       </c>
       <c r="F56" s="96">
         <f>SUM(F53:F55)</f>
-        <v>-181036.93000000005</v>
+        <v>-198316.10999999975</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="509">
+      <c r="K56" s="510">
         <f>-C4</f>
         <v>-1149740.4099999999</v>
       </c>
-      <c r="L56" s="510"/>
+      <c r="L56" s="511"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -37931,22 +37978,22 @@
       <c r="C58" s="112">
         <v>44619</v>
       </c>
-      <c r="D58" s="487" t="s">
+      <c r="D58" s="488" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="488"/>
+      <c r="E58" s="489"/>
       <c r="F58" s="113">
         <v>1266568.45</v>
       </c>
-      <c r="I58" s="489" t="s">
-        <v>198</v>
-      </c>
-      <c r="J58" s="490"/>
-      <c r="K58" s="491">
+      <c r="I58" s="490" t="s">
+        <v>97</v>
+      </c>
+      <c r="J58" s="491"/>
+      <c r="K58" s="492">
         <f>K54+K56</f>
-        <v>15504.110000000102</v>
-      </c>
-      <c r="L58" s="491"/>
+        <v>-1775.0699999995995</v>
+      </c>
+      <c r="L58" s="492"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>

</xml_diff>

<commit_message>
CIERRE 31 MAR 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #03  MARZO  2022/BALANCE    ZAVALETA   MARZO  2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #03  MARZO  2022/BALANCE    ZAVALETA   MARZO  2022.xlsx
@@ -457,7 +457,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="594">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -2224,6 +2224,21 @@
   </si>
   <si>
     <t>QUESOS-JAMONES-POLLO</t>
+  </si>
+  <si>
+    <t>SALCHICHAS JAMON ENCHILADA-POLLO</t>
+  </si>
+  <si>
+    <t>NOMINA # 12</t>
+  </si>
+  <si>
+    <t>SALCHICHONERIA -JAMON-QUESO</t>
+  </si>
+  <si>
+    <t>CHORIZO-LONGANIZA-QUESO</t>
+  </si>
+  <si>
+    <t>CHORIZO-POLLO-MIXIOTES-NUGETS-BONELES-PAPAS</t>
   </si>
 </sst>
 </file>
@@ -4123,7 +4138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="598">
+  <cellXfs count="597">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -5431,7 +5446,6 @@
     <xf numFmtId="44" fontId="11" fillId="14" borderId="99" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="6" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -13102,8 +13116,8 @@
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="J6" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13123,7 +13137,7 @@
     <col min="14" max="14" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.85546875" customWidth="1"/>
-    <col min="17" max="17" width="18.140625" style="225" customWidth="1"/>
+    <col min="17" max="17" width="21.28515625" style="225" customWidth="1"/>
     <col min="18" max="18" width="15.28515625" style="227" customWidth="1"/>
     <col min="19" max="20" width="11.42578125" customWidth="1"/>
     <col min="21" max="21" width="15.85546875" style="1" customWidth="1"/>
@@ -14163,20 +14177,20 @@
       <c r="J22" s="37"/>
       <c r="K22" s="31"/>
       <c r="L22" s="49"/>
-      <c r="M22" s="182">
-        <f>642</f>
-        <v>642</v>
+      <c r="M22" s="32">
+        <f>642+62879</f>
+        <v>63521</v>
       </c>
       <c r="N22" s="33">
         <v>23356</v>
       </c>
       <c r="P22" s="39">
         <f t="shared" si="0"/>
-        <v>48400</v>
-      </c>
-      <c r="Q22" s="597">
-        <f t="shared" si="1"/>
-        <v>-62879</v>
+        <v>111279</v>
+      </c>
+      <c r="Q22" s="326">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="R22" s="320">
         <v>0</v>
@@ -14214,19 +14228,19 @@
       <c r="J23" s="50"/>
       <c r="K23" s="172"/>
       <c r="L23" s="45"/>
-      <c r="M23" s="182">
-        <v>0</v>
+      <c r="M23" s="32">
+        <v>53950</v>
       </c>
       <c r="N23" s="33">
         <v>26005</v>
       </c>
       <c r="P23" s="39">
         <f t="shared" si="0"/>
-        <v>41339</v>
+        <v>95289</v>
       </c>
       <c r="Q23" s="326">
         <f t="shared" si="1"/>
-        <v>-53950</v>
+        <v>0</v>
       </c>
       <c r="R23" s="320">
         <v>0</v>
@@ -14242,33 +14256,47 @@
       <c r="B24" s="24">
         <v>44639</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="42"/>
+      <c r="C24" s="25">
+        <v>10938</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>589</v>
+      </c>
       <c r="E24" s="27">
         <v>44639</v>
       </c>
-      <c r="F24" s="28"/>
+      <c r="F24" s="28">
+        <v>117091</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="36">
         <v>44639</v>
       </c>
-      <c r="I24" s="30"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="173"/>
-      <c r="L24" s="52"/>
+      <c r="I24" s="30">
+        <v>2386</v>
+      </c>
+      <c r="J24" s="51">
+        <v>44639</v>
+      </c>
+      <c r="K24" s="173" t="s">
+        <v>590</v>
+      </c>
+      <c r="L24" s="52">
+        <v>20799.990000000002</v>
+      </c>
       <c r="M24" s="32">
-        <v>0</v>
+        <v>28076</v>
       </c>
       <c r="N24" s="33">
-        <v>0</v>
+        <v>54891</v>
       </c>
       <c r="P24" s="39">
         <f>N24+M24+L24+I24+C24</f>
-        <v>0</v>
+        <v>117090.99</v>
       </c>
       <c r="Q24" s="326">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-9.9999999947613105E-3</v>
       </c>
       <c r="R24" s="320">
         <v>0</v>
@@ -14284,29 +14312,37 @@
       <c r="B25" s="24">
         <v>44640</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="35"/>
+      <c r="C25" s="25">
+        <v>8565</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>591</v>
+      </c>
       <c r="E25" s="27">
         <v>44640</v>
       </c>
-      <c r="F25" s="28"/>
+      <c r="F25" s="28">
+        <v>78608</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="36">
         <v>44640</v>
       </c>
-      <c r="I25" s="30"/>
+      <c r="I25" s="30">
+        <v>1272.5</v>
+      </c>
       <c r="J25" s="50"/>
       <c r="K25" s="38"/>
       <c r="L25" s="54"/>
       <c r="M25" s="32">
-        <v>0</v>
+        <v>47560.5</v>
       </c>
       <c r="N25" s="33">
-        <v>0</v>
+        <v>21210</v>
       </c>
       <c r="P25" s="283">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>78608</v>
       </c>
       <c r="Q25" s="326">
         <f t="shared" si="1"/>
@@ -14325,30 +14361,38 @@
       <c r="B26" s="24">
         <v>44641</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="35"/>
+      <c r="C26" s="25">
+        <v>16233</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>592</v>
+      </c>
       <c r="E26" s="27">
         <v>44641</v>
       </c>
-      <c r="F26" s="28"/>
+      <c r="F26" s="28">
+        <v>95964</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="36">
         <v>44641</v>
       </c>
-      <c r="I26" s="30"/>
+      <c r="I26" s="30">
+        <v>843</v>
+      </c>
       <c r="J26" s="37"/>
       <c r="K26" s="173"/>
       <c r="L26" s="45"/>
       <c r="M26" s="32">
-        <v>0</v>
+        <v>36536</v>
       </c>
       <c r="N26" s="33">
-        <v>0</v>
+        <v>42352</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" s="284">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>95964</v>
       </c>
       <c r="Q26" s="326">
         <f t="shared" si="1"/>
@@ -14367,37 +14411,44 @@
       <c r="B27" s="24">
         <v>44642</v>
       </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="42"/>
+      <c r="C27" s="25">
+        <v>14717</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>593</v>
+      </c>
       <c r="E27" s="27">
         <v>44642</v>
       </c>
-      <c r="F27" s="28"/>
+      <c r="F27" s="28">
+        <v>92410</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="36">
         <v>44642</v>
       </c>
-      <c r="I27" s="30"/>
+      <c r="I27" s="30">
+        <v>563.5</v>
+      </c>
       <c r="J27" s="55"/>
       <c r="K27" s="174"/>
       <c r="L27" s="54"/>
       <c r="M27" s="32">
-        <v>0</v>
+        <v>42310.5</v>
       </c>
       <c r="N27" s="33">
-        <v>0</v>
+        <v>34989</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>92580</v>
       </c>
       <c r="Q27" s="326">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R27" s="320">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="R27" s="406">
+        <v>170</v>
       </c>
       <c r="W27" s="542"/>
       <c r="X27" s="543"/>
@@ -14716,12 +14767,10 @@
       <c r="N35" s="268">
         <v>0</v>
       </c>
-      <c r="P35" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q35" s="438" t="e">
+      <c r="P35" s="34"/>
+      <c r="Q35" s="111">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
       <c r="R35" s="228"/>
     </row>
@@ -14746,19 +14795,19 @@
       <c r="L36" s="44"/>
       <c r="M36" s="533">
         <f>SUM(M5:M35)</f>
-        <v>802713.66</v>
+        <v>1074025.6600000001</v>
       </c>
       <c r="N36" s="535">
         <f>SUM(N5:N35)</f>
-        <v>523841</v>
+        <v>677283</v>
       </c>
       <c r="O36" s="276"/>
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="571" t="e">
+      <c r="Q36" s="571">
         <f>SUM(Q5:Q35)</f>
-        <v>#VALUE!</v>
+        <v>1.5800000000308501</v>
       </c>
       <c r="R36" s="228"/>
     </row>
@@ -14839,12 +14888,12 @@
       <c r="L39" s="61"/>
       <c r="M39" s="573">
         <f>M36+N36</f>
-        <v>1326554.6600000001</v>
+        <v>1751308.6600000001</v>
       </c>
       <c r="N39" s="574"/>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
-        <v>1721480.59</v>
+        <v>2222552.58</v>
       </c>
       <c r="Q39" s="275"/>
     </row>
@@ -14924,9 +14973,15 @@
       <c r="G43" s="2"/>
       <c r="H43" s="76"/>
       <c r="I43" s="77"/>
-      <c r="J43" s="50"/>
-      <c r="K43" s="38"/>
-      <c r="L43" s="54"/>
+      <c r="J43" s="50">
+        <v>44639</v>
+      </c>
+      <c r="K43" s="38" t="s">
+        <v>590</v>
+      </c>
+      <c r="L43" s="54">
+        <v>14398.5</v>
+      </c>
       <c r="M43" s="269"/>
       <c r="N43" s="269"/>
       <c r="P43" s="34"/>
@@ -15047,7 +15102,7 @@
       </c>
       <c r="C50" s="87">
         <f>SUM(C5:C49)</f>
-        <v>296745</v>
+        <v>347198</v>
       </c>
       <c r="D50" s="88"/>
       <c r="E50" s="89" t="s">
@@ -15055,7 +15110,7 @@
       </c>
       <c r="F50" s="90">
         <f>SUM(F5:F49)</f>
-        <v>1796139</v>
+        <v>2180212</v>
       </c>
       <c r="G50" s="88"/>
       <c r="H50" s="91" t="s">
@@ -15063,7 +15118,7 @@
       </c>
       <c r="I50" s="92">
         <f>SUM(I5:I49)</f>
-        <v>68017.5</v>
+        <v>73082.5</v>
       </c>
       <c r="J50" s="93"/>
       <c r="K50" s="94" t="s">
@@ -15071,7 +15126,7 @@
       </c>
       <c r="L50" s="95">
         <f>SUM(L5:L49)</f>
-        <v>61107.19</v>
+        <v>96305.68</v>
       </c>
       <c r="M50" s="96"/>
       <c r="N50" s="96"/>
@@ -15096,7 +15151,7 @@
       <c r="J52" s="100"/>
       <c r="K52" s="512">
         <f>I50+L50</f>
-        <v>129124.69</v>
+        <v>169388.18</v>
       </c>
       <c r="L52" s="539"/>
       <c r="M52" s="272"/>
@@ -15111,7 +15166,7 @@
       <c r="E53" s="516"/>
       <c r="F53" s="313">
         <f>F50-K52-C50</f>
-        <v>1370269.31</v>
+        <v>1663625.82</v>
       </c>
       <c r="I53" s="102"/>
       <c r="J53" s="103"/>
@@ -15130,7 +15185,7 @@
       <c r="J54" s="518"/>
       <c r="K54" s="519">
         <f>F56+F57+F58</f>
-        <v>1370269.31</v>
+        <v>1663625.82</v>
       </c>
       <c r="L54" s="519"/>
       <c r="M54" s="422"/>
@@ -15166,7 +15221,7 @@
       </c>
       <c r="F56" s="96">
         <f>SUM(F53:F55)</f>
-        <v>1370269.31</v>
+        <v>1663625.82</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="108" t="s">
@@ -15207,7 +15262,7 @@
       <c r="J58" s="502"/>
       <c r="K58" s="503">
         <f>K54+K56</f>
-        <v>103700.8600000001</v>
+        <v>397057.37000000011</v>
       </c>
       <c r="L58" s="503"/>
     </row>

</xml_diff>